<commit_message>
Updated the second version of the energy monitoring template with tileviews
</commit_message>
<xml_diff>
--- a/_templates/Energy-Monitoring-ISO-50001/Energymonitoring.xlsx
+++ b/_templates/Energy-Monitoring-ISO-50001/Energymonitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyanova\Documents\GitHub\peakboard-templates.github.io\_templates\Energy-Monitoring-ISO-50001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE85ED5-0B53-4FED-A26D-65BD94B22D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643A4A39-D876-40D7-B961-C6211C8B33C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1725" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{F096A637-B66B-484B-A9AD-CFB9F8633A2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F096A637-B66B-484B-A9AD-CFB9F8633A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Engine" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>y</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Turned on</t>
   </si>
 </sst>
 </file>
@@ -408,37 +417,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C90CC00-5F88-4A86-8F02-9595081EE0DB}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -449,39 +475,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D03FC3-CCC3-45D4-BF65-0D198D01C33B}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="A6" sqref="A6:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>777</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2270</v>
-      </c>
-      <c r="D2">
+      <c r="B5">
         <v>0</v>
       </c>
     </row>
@@ -498,12 +539,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -520,7 +561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.4375</v>
       </c>
@@ -537,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.44097222222222227</v>
       </c>
@@ -554,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.44444444444444442</v>
       </c>
@@ -571,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.44791666666666669</v>
       </c>
@@ -588,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.45138888888888901</v>
       </c>
@@ -605,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.45486111111111099</v>
       </c>
@@ -622,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.45833333333333398</v>
       </c>
@@ -639,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.46180555555555602</v>
       </c>
@@ -656,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.46527777777777801</v>
       </c>
@@ -673,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.46875</v>
       </c>
@@ -690,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.47222222222222299</v>
       </c>
@@ -707,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.47569444444444497</v>
       </c>
@@ -724,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.47916666666666702</v>
       </c>

</xml_diff>

<commit_message>
Removed unneccessary data and files, adjusted the template
</commit_message>
<xml_diff>
--- a/_templates/Energy-Monitoring-ISO-50001/Energymonitoring.xlsx
+++ b/_templates/Energy-Monitoring-ISO-50001/Energymonitoring.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyanova\Documents\GitHub\peakboard-templates.github.io\_templates\Energy-Monitoring-ISO-50001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643A4A39-D876-40D7-B961-C6211C8B33C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EDD185-CB9F-40F0-ABB3-53BB96E3159B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F096A637-B66B-484B-A9AD-CFB9F8633A2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F096A637-B66B-484B-A9AD-CFB9F8633A2D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Engine" sheetId="1" r:id="rId1"/>
-    <sheet name="Air Volume" sheetId="2" r:id="rId2"/>
-    <sheet name="Energy Consumption" sheetId="3" r:id="rId3"/>
+    <sheet name="Air Volume" sheetId="2" r:id="rId1"/>
+    <sheet name="Energy Consumption" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Compressor 1</t>
   </si>
@@ -58,13 +51,22 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Compressor</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
-    <t>Turned on</t>
+    <t>VD 1</t>
+  </si>
+  <si>
+    <t>VD 2</t>
+  </si>
+  <si>
+    <t>VD 3</t>
+  </si>
+  <si>
+    <t>VD 4</t>
+  </si>
+  <si>
+    <t>VD</t>
   </si>
 </sst>
 </file>
@@ -416,70 +418,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C90CC00-5F88-4A86-8F02-9595081EE0DB}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D03FC3-CCC3-45D4-BF65-0D198D01C33B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -488,15 +430,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>777</v>
@@ -504,7 +446,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -512,7 +454,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>2270</v>
@@ -520,7 +462,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -531,12 +473,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FBA0CF-ABA4-4A11-B51A-C1E10101478D}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,19 +488,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -779,6 +721,125 @@
         <v>295</v>
       </c>
       <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0.48263888888888901</v>
+      </c>
+      <c r="B15">
+        <v>230</v>
+      </c>
+      <c r="C15">
+        <v>380</v>
+      </c>
+      <c r="D15">
+        <v>295</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>0.48611111111111099</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="C16">
+        <v>350</v>
+      </c>
+      <c r="D16">
+        <v>295</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="B17">
+        <v>210</v>
+      </c>
+      <c r="C17">
+        <v>320</v>
+      </c>
+      <c r="D17">
+        <v>295</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0.49305555555555503</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+      <c r="D18">
+        <v>295</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>0.49652777777777701</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
+        <v>150</v>
+      </c>
+      <c r="D19">
+        <v>295</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>0.499999999999999</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>295</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>0.50347222222222099</v>
+      </c>
+      <c r="B21">
+        <v>220</v>
+      </c>
+      <c r="C21">
+        <v>310</v>
+      </c>
+      <c r="D21">
+        <v>295</v>
+      </c>
+      <c r="E21">
         <v>0</v>
       </c>
     </row>

</xml_diff>